<commit_message>
EXL_CorporateLensHomePage_Alerts EXL_CorporateLensHomePage_NewsCarousel EXL_CorporateLensHomePage_Blogs EXL_CorporateLensHomePage_MyDocuments
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
+++ b/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excelens_JWS\Excelens_Trunk_Jul122017\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_EXCL_JUL\Excelens_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>TCID</t>
   </si>
@@ -48,23 +48,34 @@
     <t>EXL_CorporateLensHomePage_Alerts</t>
   </si>
   <si>
-    <t>Contributor creates an Alert and validate as visitor</t>
+    <t>EXL_CorporateLensHomePage_NewsCarousel</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_Blogs</t>
+  </si>
+  <si>
+    <t>Creates an new Alert</t>
+  </si>
+  <si>
+    <t>Creates a News Carousel</t>
+  </si>
+  <si>
+    <t>Creates a New Blog</t>
   </si>
   <si>
     <t>Sprint1</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
+    <t>EXL_CorporateLensHomePage_MyDocuments</t>
+  </si>
+  <si>
+    <t>Upload a New Document</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -487,19 +498,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="73.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -527,7 +538,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -535,19 +546,71 @@
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Included and Marked EXL_CorporateLensHomePage_MyFavourites for execution
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
+++ b/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>TCID</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Upload a New Document</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_MyFavourites</t>
+  </si>
+  <si>
+    <t>Add Favourites</t>
   </si>
 </sst>
 </file>
@@ -498,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -605,12 +611,30 @@
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D6">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Included EXL_CorporateLensHomePage_Announcements and marked for execution.
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
+++ b/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>TCID</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Add Favourites</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_Announcements</t>
+  </si>
+  <si>
+    <t>Add Announcement</t>
   </si>
 </sst>
 </file>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -629,12 +635,30 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D7">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Included and marked for execution - EXL_CorporateLensHomePage_CalendarEvent
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
+++ b/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>TCID</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Add Announcement</t>
+  </si>
+  <si>
+    <t>Add New Event in Calender</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_CalendarEvent</t>
   </si>
 </sst>
 </file>
@@ -510,11 +516,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -653,12 +657,30 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D8">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
EXL_CorporateLensHomePage_MarketPlace-Included and marked for execution.
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
+++ b/Excelens_Trunk/src/com/proj/suite/corporateLens Suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>TCID</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>EXL_CorporateLensHomePage_CalendarEvent</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_MarketPlace</t>
+  </si>
+  <si>
+    <t>Add New Marketplace</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -675,12 +681,30 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D9">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9">
       <formula1>"Sprint1,Sprint2,Sprint3,Sprint4,Sprint5,Sprint6,Sprint7,Sprint8,Sprint9,Sprint10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>